<commit_message>
add : ajout feature suppression groupée
</commit_message>
<xml_diff>
--- a/ressources/Backlog Projet Création site web RIL10.xlsx
+++ b/ressources/Backlog Projet Création site web RIL10.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\vuejs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\vuejs\vuejs_project\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>Story ID</t>
   </si>
@@ -490,7 +490,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -528,13 +528,13 @@
       <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="D2" s="9"/>
       <c r="E2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="9"/>
+      <c r="F2" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -547,7 +547,9 @@
         <v>1</v>
       </c>
       <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="E3" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="F3" s="9" t="s">
         <v>25</v>
       </c>
@@ -578,11 +580,13 @@
       <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -678,11 +682,13 @@
       <c r="C11" s="5">
         <v>3</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -694,11 +700,13 @@
       <c r="C12" s="5">
         <v>3</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">

</xml_diff>